<commit_message>
Actualización completa: simulaciones, resultados y datos base
- Actualización de sim_caso_base.py con mejoras en visualización y simulaciones
- Actualización de resultados de simulaciones (results_caso_4.xlsx, results_montecarlo.xlsx)
- Actualización de archivos base de datos (Simulacion_caso_base.xlsx, Test Dilucion.xlsx)
</commit_message>
<xml_diff>
--- a/Sims caso base/results/results_caso_4.xlsx
+++ b/Sims caso base/results/results_caso_4.xlsx
@@ -547,16 +547,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>86.5131225152</v>
+        <v>85.33359125119999</v>
       </c>
       <c r="C2" t="n">
-        <v>14.04896333</v>
+        <v>16.121362785</v>
       </c>
       <c r="D2" t="n">
-        <v>6.157971978648477</v>
+        <v>5.293199612789435</v>
       </c>
       <c r="E2" t="n">
-        <v>14.77913274875634</v>
+        <v>12.70367907069464</v>
       </c>
       <c r="F2" t="n">
         <v>24.515</v>
@@ -568,19 +568,19 @@
         <v>22.4925125</v>
       </c>
       <c r="I2" t="n">
-        <v>4.8492966246505</v>
+        <v>4.20404357200725</v>
       </c>
       <c r="J2" t="n">
         <v>22.4925125</v>
       </c>
       <c r="K2" t="n">
-        <v>6.270912485</v>
+        <v>6.13370815875</v>
       </c>
       <c r="L2" t="n">
-        <v>16.221600015</v>
+        <v>16.35880434125</v>
       </c>
       <c r="M2" t="n">
-        <v>1.4216158603495</v>
+        <v>1.92966458674275</v>
       </c>
       <c r="N2" t="n">
         <v>2.4</v>
@@ -592,19 +592,19 @@
         <v>0.8182234332425067</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.407120280898204</v>
+        <v>1.761901158124151</v>
       </c>
       <c r="R2" t="n">
         <v>0.8182234332425067</v>
       </c>
       <c r="S2" t="n">
-        <v>2.757542101415564</v>
+        <v>2.801222578933642</v>
       </c>
       <c r="T2" t="n">
-        <v>0.06852564526878455</v>
+        <v>0.0747009981676096</v>
       </c>
       <c r="U2" t="n">
-        <v>7.363987596810685</v>
+        <v>5.065529323443576</v>
       </c>
     </row>
   </sheetData>
@@ -738,16 +738,16 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>96.56816282777024</v>
+        <v>95.78052290468307</v>
       </c>
       <c r="C2" t="n">
-        <v>17.58497919765321</v>
+        <v>19.82325696100919</v>
       </c>
       <c r="D2" t="n">
-        <v>5.491514191876761</v>
+        <v>4.831724831750702</v>
       </c>
       <c r="E2" t="n">
-        <v>13.17963406050423</v>
+        <v>11.59613959620168</v>
       </c>
       <c r="F2" t="n">
         <v>24.515</v>
@@ -759,19 +759,19 @@
         <v>21.8943465</v>
       </c>
       <c r="I2" t="n">
-        <v>5.765823552847874</v>
+        <v>4.878013028644973</v>
       </c>
       <c r="J2" t="n">
-        <v>26.7436431246505</v>
+        <v>26.09839007200725</v>
       </c>
       <c r="K2" t="n">
-        <v>7.45612770315256</v>
+        <v>7.117030972636377</v>
       </c>
       <c r="L2" t="n">
-        <v>19.28751542149794</v>
+        <v>18.98135909937088</v>
       </c>
       <c r="M2" t="n">
-        <v>1.690304150304685</v>
+        <v>2.239017943991404</v>
       </c>
       <c r="N2" t="n">
         <v>2.4</v>
@@ -783,19 +783,19 @@
         <v>0.6250587840107491</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.318799981474386</v>
+        <v>1.740288072173941</v>
       </c>
       <c r="R2" t="n">
-        <v>0.7668662467954221</v>
+        <v>0.8081863586270529</v>
       </c>
       <c r="S2" t="n">
-        <v>2.584460277937513</v>
+        <v>2.766860228875015</v>
       </c>
       <c r="T2" t="n">
-        <v>0.06422451650921174</v>
+        <v>0.07378464761836426</v>
       </c>
       <c r="U2" t="n">
-        <v>6.901774381399957</v>
+        <v>5.003390922463434</v>
       </c>
     </row>
   </sheetData>
@@ -929,64 +929,64 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>83.33565667950711</v>
+        <v>87.40324667284139</v>
       </c>
       <c r="C2" t="n">
-        <v>11.92882878689641</v>
+        <v>15.77147756935734</v>
       </c>
       <c r="D2" t="n">
-        <v>6.986071991497584</v>
+        <v>5.541855307371997</v>
       </c>
       <c r="E2" t="n">
-        <v>16.7665727795942</v>
+        <v>13.30045273769279</v>
       </c>
       <c r="F2" t="n">
         <v>24.515</v>
       </c>
       <c r="G2" t="n">
-        <v>1.07866</v>
+        <v>1.4709</v>
       </c>
       <c r="H2" t="n">
-        <v>23.43634</v>
+        <v>23.0441</v>
       </c>
       <c r="I2" t="n">
-        <v>6.295870821426332</v>
+        <v>5.218882496783531</v>
       </c>
       <c r="J2" t="n">
-        <v>29.20216355284787</v>
+        <v>27.92211302864497</v>
       </c>
       <c r="K2" t="n">
-        <v>8.141563198533987</v>
+        <v>7.614360222911484</v>
       </c>
       <c r="L2" t="n">
-        <v>21.06060035431389</v>
+        <v>20.30775280573349</v>
       </c>
       <c r="M2" t="n">
-        <v>1.845692377107655</v>
+        <v>2.395477726127953</v>
       </c>
       <c r="N2" t="n">
         <v>2.4</v>
       </c>
       <c r="O2" t="n">
-        <v>24.16363636363636</v>
+        <v>22.716</v>
       </c>
       <c r="P2" t="n">
-        <v>1.398326359832636</v>
+        <v>1.103234042553192</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.377735186703753</v>
+        <v>2.615273423367069</v>
       </c>
       <c r="R2" t="n">
-        <v>1.382624267603036</v>
+        <v>1.21452783515595</v>
       </c>
       <c r="S2" t="n">
-        <v>4.659661986512956</v>
+        <v>4.157987484054254</v>
       </c>
       <c r="T2" t="n">
-        <v>0.1157938238536098</v>
+        <v>0.1108822332659908</v>
       </c>
       <c r="U2" t="n">
-        <v>12.44357903235529</v>
+        <v>7.519005339092387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>